<commit_message>
finished first draft of outline and re-named figures
</commit_message>
<xml_diff>
--- a/manuscript /meso_tx_table.xlsx
+++ b/manuscript /meso_tx_table.xlsx
@@ -31,10 +31,10 @@
     <t>%tx</t>
   </si>
   <si>
-    <t>total crypto SF</t>
-  </si>
-  <si>
-    <t>Tx # SF</t>
+    <t>total crypto SF/mL</t>
+  </si>
+  <si>
+    <t>Tx # SF/mL</t>
   </si>
 </sst>
 </file>
@@ -49,6 +49,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -110,10 +111,11 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -131,18 +133,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="1">
@@ -161,7 +163,7 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -200,8 +202,13 @@
       <c r="D4" s="0" t="n">
         <v>0.1788893</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>0.075166434</v>
+      <c r="E4" s="3" t="n">
+        <f aca="false">(75166.434)/1000</f>
+        <v>75.166434</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">D4*E4</f>
+        <v>13.4464707617562</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="5">
@@ -275,8 +282,13 @@
       <c r="D10" s="0" t="n">
         <v>0.0801162</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>0.35278684</v>
+      <c r="E10" s="3" t="n">
+        <f aca="false">(352786.84)/1000</f>
+        <v>352.78684</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">D10*E10</f>
+        <v>28.263941030808</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="11">
@@ -377,17 +389,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -402,17 +414,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
improving a few figures and working on paper
</commit_message>
<xml_diff>
--- a/manuscript /meso_tx_table.xlsx
+++ b/manuscript /meso_tx_table.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Tx # SF/mL</t>
+  </si>
+  <si>
+    <t>total crypto SF/mL weekly mean</t>
+  </si>
+  <si>
+    <t>Tx # SF/mL new</t>
   </si>
 </sst>
 </file>
@@ -133,18 +139,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="H16" activeCellId="0" pane="topLeft" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6078431372549"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9803921568627"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.0235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.3529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="1">
@@ -166,6 +175,12 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="2">
       <c r="A2" s="1" t="n">
@@ -202,7 +217,7 @@
       <c r="D4" s="0" t="n">
         <v>0.1788893</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="0" t="n">
         <f aca="false">(75166.434)/1000</f>
         <v>75.166434</v>
       </c>
@@ -210,6 +225,14 @@
         <f aca="false">D4*E4</f>
         <v>13.4464707617562</v>
       </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false">(520876.1/1000)</f>
+        <v>520.8761</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">(0.1788893*G4)</f>
+        <v>93.17916091573</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="5">
       <c r="A5" s="1" t="n">
@@ -257,6 +280,14 @@
       <c r="D8" s="0" t="n">
         <v>0.0615413</v>
       </c>
+      <c r="G8" s="3" t="n">
+        <f aca="false">(81760.8/1000)</f>
+        <v>81.7608</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">(D8*G8)</f>
+        <v>5.03166592104</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="9">
       <c r="A9" s="1" t="n">
@@ -282,7 +313,7 @@
       <c r="D10" s="0" t="n">
         <v>0.0801162</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="0" t="n">
         <f aca="false">(352786.84)/1000</f>
         <v>352.78684</v>
       </c>
@@ -290,6 +321,14 @@
         <f aca="false">D10*E10</f>
         <v>28.263941030808</v>
       </c>
+      <c r="G10" s="3" t="n">
+        <f aca="false">(94497.04/1000)</f>
+        <v>94.49704</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">D10*G10</f>
+        <v>7.570743756048</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="11">
       <c r="A11" s="1" t="n">
@@ -347,6 +386,14 @@
       </c>
       <c r="D15" s="0" t="n">
         <v>0.2281905</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <f aca="false">(236434.8/1000)</f>
+        <v>236.4348</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">D15*G15</f>
+        <v>53.9521752294</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="16">
@@ -394,7 +441,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -419,7 +466,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>